<commit_message>
I think I improved this programm
</commit_message>
<xml_diff>
--- a/wrong1.xlsx
+++ b/wrong1.xlsx
@@ -417,7 +417,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,12 +499,8 @@
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4">
-        <v>14</v>
-      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="4">
         <v>15</v>
       </c>
@@ -517,7 +513,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="4">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D7" s="4">
         <v>18</v>

</xml_diff>